<commit_message>
successfully calculated quartz hugoniot
</commit_message>
<xml_diff>
--- a/MgO_hugoniot.xlsx
+++ b/MgO_hugoniot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixuanye/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitris/PycharmProjects/MSEE_MgO_UQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C042471F-3CC9-2A42-978F-698C59BABF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76FDB88-38E5-E549-A41A-575193E4F06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="1680" windowWidth="27240" windowHeight="16040" xr2:uid="{D46272E7-0D86-2B4A-9EF5-9922D59D6814}"/>
+    <workbookView xWindow="67000" yWindow="0" windowWidth="20040" windowHeight="28800" activeTab="5" xr2:uid="{D46272E7-0D86-2B4A-9EF5-9922D59D6814}"/>
   </bookViews>
   <sheets>
     <sheet name="MgO" sheetId="1" r:id="rId1"/>
@@ -113,19 +113,19 @@
     <t xml:space="preserve">Pressure_Error (GPa) </t>
   </si>
   <si>
-    <t xml:space="preserve">Pressure (GPa) </t>
-  </si>
-  <si>
-    <t>Us (km/s)</t>
-  </si>
-  <si>
     <t>destination_Us</t>
   </si>
   <si>
     <t>Us</t>
   </si>
   <si>
-    <t>err</t>
+    <t>errUs</t>
+  </si>
+  <si>
+    <t>errUp</t>
+  </si>
+  <si>
+    <t>errP</t>
   </si>
 </sst>
 </file>
@@ -1842,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8479150D-6A50-1D46-8FA1-E10B4FE01773}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3682,24 +3682,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2AA4F0-56F4-3749-997C-EFB07B902B6A}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -5342,7 +5342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDA244C-BE22-F743-B543-0658EB5BBD1E}">
   <dimension ref="A1:I162"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
@@ -8536,7 +8536,7 @@
         <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -10286,7 +10286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E81ECD2-539B-424B-940D-F4C8FD6E8D5D}">
   <dimension ref="A1:D196"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -12460,8 +12460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C93E3A8-78DD-8447-85BD-FCD88225569A}">
   <dimension ref="A1:F203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12484,7 +12484,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>23</v>

</xml_diff>